<commit_message>
update run sensitivity to take values from excel
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52A7B87-9950-433B-BAD6-0A65CD1C5FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BC671D-781A-429A-A060-86CF052F45C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="105">
   <si>
     <t>Mh</t>
   </si>
@@ -129,9 +129,6 @@
     <t>E_ROSh</t>
   </si>
   <si>
-    <t>VROSmax</t>
-  </si>
-  <si>
     <t>K_ROSh</t>
   </si>
   <si>
@@ -198,24 +195,12 @@
     <t>description</t>
   </si>
   <si>
-    <t>death rate</t>
-  </si>
-  <si>
-    <t>% of recyclable dead matter (rest goes to recalcitrant)</t>
-  </si>
-  <si>
     <t>C:N ratio</t>
   </si>
   <si>
-    <t>leakage rate</t>
-  </si>
-  <si>
     <t>µmol/L</t>
   </si>
   <si>
-    <t>maximum uptake rate</t>
-  </si>
-  <si>
     <t>µmol/L/sec</t>
   </si>
   <si>
@@ -297,9 +282,6 @@
     <t>logscale fitting</t>
   </si>
   <si>
-    <t>K’s (affinity), half-velocity constant (0.17 * organism_volume**0.27)</t>
-  </si>
-  <si>
     <t>LEAK model hardcoded parameters</t>
   </si>
   <si>
@@ -325,6 +307,51 @@
   </si>
   <si>
     <t>ROS</t>
+  </si>
+  <si>
+    <t>HET death rate</t>
+  </si>
+  <si>
+    <t>PRO death rate</t>
+  </si>
+  <si>
+    <t>% of recyclable dead matter of PRO (rest goes to recalcitrant)</t>
+  </si>
+  <si>
+    <t>% of recyclable dead matter of HET (rest goes to recalcitrant)</t>
+  </si>
+  <si>
+    <t>organic leakage rate</t>
+  </si>
+  <si>
+    <t>inorganic leakage rate</t>
+  </si>
+  <si>
+    <t>organic N K’s (affinity), half-velocity constant (0.17 * organism_volume**0.27)</t>
+  </si>
+  <si>
+    <t>inorganic N K’s (affinity), half-velocity constant (0.17 * organism_volume**0.27)</t>
+  </si>
+  <si>
+    <t>organic C K’s (affinity), half-velocity constant (0.17 * organism_volume**0.27)</t>
+  </si>
+  <si>
+    <t>inorganic C K’s (affinity), half-velocity constant (0.17 * organism_volume**0.27)</t>
+  </si>
+  <si>
+    <t>organic N maximum uptake rate</t>
+  </si>
+  <si>
+    <t>inorganic N maximum uptake rate</t>
+  </si>
+  <si>
+    <t>organic C maximum uptake rate</t>
+  </si>
+  <si>
+    <t>inorganic C maximum uptake rate</t>
+  </si>
+  <si>
+    <t>VmaxROSh</t>
   </si>
 </sst>
 </file>
@@ -913,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,7 +949,7 @@
     <col min="1" max="1" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="66.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
@@ -934,46 +961,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="29" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>48</v>
-      </c>
       <c r="C1" s="27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="N1" s="29" t="s">
         <v>80</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="K1" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="M1" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="N1" s="29" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -981,13 +1008,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E2" s="14">
         <v>1.157407407407407E-6</v>
@@ -997,10 +1024,21 @@
         <v>9.999999999999995E-2</v>
       </c>
       <c r="J2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K2" t="s">
-        <v>81</v>
+        <v>76</v>
+      </c>
+      <c r="L2" s="5">
+        <f>E2/10</f>
+        <v>1.157407407407407E-7</v>
+      </c>
+      <c r="M2" s="5">
+        <f>E2*100</f>
+        <v>1.1574074074074069E-4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1008,13 +1046,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E3" s="6">
         <v>1.157407407407407E-6</v>
@@ -1024,10 +1062,21 @@
         <v>9.999999999999995E-2</v>
       </c>
       <c r="J3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K3" t="s">
-        <v>81</v>
+        <v>76</v>
+      </c>
+      <c r="L3" s="5">
+        <f>E3/10</f>
+        <v>1.157407407407407E-7</v>
+      </c>
+      <c r="M3" s="5">
+        <f>E3*100</f>
+        <v>1.1574074074074069E-4</v>
+      </c>
+      <c r="N3" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1035,23 +1084,23 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E4" s="7">
         <v>0.6</v>
       </c>
       <c r="F4" s="17"/>
       <c r="J4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1060,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1068,23 +1117,23 @@
         <v>3</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E5" s="20">
         <v>0.6</v>
       </c>
       <c r="F5" s="21"/>
       <c r="J5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -1093,7 +1142,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1101,23 +1150,23 @@
         <v>4</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E6" s="22">
         <v>7</v>
       </c>
       <c r="F6" s="15"/>
       <c r="J6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1125,23 +1174,23 @@
         <v>5</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E7" s="20">
         <v>4.5</v>
       </c>
       <c r="F7" s="21"/>
       <c r="J7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1149,13 +1198,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E8" s="14">
         <v>1.157407407407407E-6</v>
@@ -1168,10 +1217,10 @@
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1181,21 +1230,21 @@
         <v>1.157407407407407E-5</v>
       </c>
       <c r="N8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E9" s="7">
         <v>0</v>
@@ -1214,10 +1263,10 @@
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1225,13 +1274,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E10" s="6">
         <v>1.157407407407407E-6</v>
@@ -1244,10 +1293,10 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1257,7 +1306,7 @@
         <v>1.157407407407407E-5</v>
       </c>
       <c r="N10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1265,13 +1314,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E11" s="20">
         <v>0</v>
@@ -1290,10 +1339,10 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K11" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1301,13 +1350,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E12" s="25">
         <v>0.1427507995452611</v>
@@ -1323,10 +1372,10 @@
       </c>
       <c r="I12" s="4"/>
       <c r="J12" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L12">
         <f>E12/10</f>
@@ -1337,7 +1386,7 @@
         <v>1.4275079954526109</v>
       </c>
       <c r="N12" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1345,23 +1394,23 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E13" s="10">
         <v>0.1427507995452611</v>
       </c>
       <c r="F13" s="17"/>
       <c r="J13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L13">
         <f t="shared" ref="L13:L19" si="1">E13/10</f>
@@ -1372,7 +1421,7 @@
         <v>1.4275079954526109</v>
       </c>
       <c r="N13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1380,13 +1429,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E14" s="10">
         <v>0.1427507995452611</v>
@@ -1401,10 +1450,10 @@
         <v>0.1427507995452611</v>
       </c>
       <c r="J14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K14" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
@@ -1415,7 +1464,7 @@
         <v>1.4275079954526109</v>
       </c>
       <c r="N14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1423,23 +1472,23 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E15" s="10">
         <v>0.1427507995452611</v>
       </c>
       <c r="F15" s="17"/>
       <c r="J15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
@@ -1450,7 +1499,7 @@
         <v>1.4275079954526109</v>
       </c>
       <c r="N15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1458,23 +1507,23 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E16" s="10">
         <v>0.2502723352076287</v>
       </c>
       <c r="F16" s="17"/>
       <c r="J16" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L16">
         <f t="shared" si="1"/>
@@ -1485,7 +1534,7 @@
         <v>2.5027233520762868</v>
       </c>
       <c r="N16" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1493,23 +1542,23 @@
         <v>15</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E17" s="10">
         <v>0.2502723352076287</v>
       </c>
       <c r="F17" s="17"/>
       <c r="J17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
@@ -1520,7 +1569,7 @@
         <v>2.5027233520762868</v>
       </c>
       <c r="N17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1528,23 +1577,23 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E18" s="10">
         <v>0.2502723352076287</v>
       </c>
       <c r="F18" s="17"/>
       <c r="J18" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K18" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L18">
         <f t="shared" si="1"/>
@@ -1555,7 +1604,7 @@
         <v>2.5027233520762868</v>
       </c>
       <c r="N18" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1563,13 +1612,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E19" s="10">
         <v>0.2502723352076287</v>
@@ -1588,10 +1637,10 @@
         <v>0.2502723352076287</v>
       </c>
       <c r="J19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
@@ -1602,7 +1651,7 @@
         <v>2.5027233520762868</v>
       </c>
       <c r="N19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1610,13 +1659,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E20" s="6">
         <f>E21/5</f>
@@ -1633,10 +1682,10 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K20" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L20">
         <f t="shared" ref="L20" si="3">E20/10</f>
@@ -1647,7 +1696,7 @@
         <v>1.6203703703703704E-5</v>
       </c>
       <c r="N20" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1655,13 +1704,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E21" s="6">
         <v>8.101851851851852E-6</v>
@@ -1671,10 +1720,10 @@
         <v>0.7</v>
       </c>
       <c r="J21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K21" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L21">
         <f>E21/10</f>
@@ -1685,7 +1734,7 @@
         <v>8.1018518518518516E-5</v>
       </c>
       <c r="N21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1693,13 +1742,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E22" s="6">
         <f>E23/5</f>
@@ -1716,10 +1765,10 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K22" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L22">
         <f>E22/10</f>
@@ -1730,7 +1779,7 @@
         <v>1.1342592592592592E-4</v>
       </c>
       <c r="N22" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1738,13 +1787,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E23" s="6">
         <v>5.6712962962962959E-5</v>
@@ -1754,10 +1803,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="J23" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K23" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L23">
         <f t="shared" ref="L23:L26" si="5">E23/10</f>
@@ -1768,7 +1817,7 @@
         <v>5.6712962962962956E-4</v>
       </c>
       <c r="N23" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1776,13 +1825,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E24" s="6">
         <v>1.50462962962963E-5</v>
@@ -1792,10 +1841,10 @@
         <v>1.3000000000000003</v>
       </c>
       <c r="J24" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K24" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L24">
         <f t="shared" si="5"/>
@@ -1806,7 +1855,7 @@
         <v>1.50462962962963E-4</v>
       </c>
       <c r="N24" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -1814,13 +1863,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E25" s="6">
         <v>1.50462962962963E-5</v>
@@ -1830,10 +1879,10 @@
         <v>1.3000000000000003</v>
       </c>
       <c r="J25" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L25">
         <f t="shared" si="5"/>
@@ -1844,7 +1893,7 @@
         <v>1.50462962962963E-4</v>
       </c>
       <c r="N25" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -1852,13 +1901,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E26" s="6">
         <v>6.7708333333333344E-5</v>
@@ -1868,10 +1917,10 @@
         <v>5.8500000000000014</v>
       </c>
       <c r="J26" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L26">
         <f t="shared" si="5"/>
@@ -1882,7 +1931,7 @@
         <v>6.7708333333333346E-4</v>
       </c>
       <c r="N26" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1890,13 +1939,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>58</v>
+        <v>48</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E27" s="20">
         <v>0</v>
@@ -1915,10 +1964,10 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K27" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -1926,13 +1975,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E28" s="22">
         <v>1</v>
@@ -1948,10 +1997,10 @@
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K28" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1959,13 +2008,13 @@
         <v>27</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E29" s="20">
         <v>1</v>
@@ -1981,10 +2030,10 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K29" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -1992,13 +2041,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E30" s="14">
         <v>6.4814814814814812E-7</v>
@@ -2017,10 +2066,10 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K30" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L30" s="5">
         <f>E30/10</f>
@@ -2031,7 +2080,7 @@
         <v>6.4814814814814812E-6</v>
       </c>
       <c r="N30" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -2039,13 +2088,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E31" s="6">
         <v>4.0509259259259258E-7</v>
@@ -2064,10 +2113,10 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K31" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L31" s="5">
         <f>E31/10</f>
@@ -2078,21 +2127,21 @@
         <v>4.050925925925926E-6</v>
       </c>
       <c r="N31" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E32" s="6">
         <v>7.6967592592592601E-6</v>
@@ -2111,10 +2160,10 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L32" s="5">
         <f t="shared" ref="L32:L35" si="7">E32/10</f>
@@ -2125,21 +2174,21 @@
         <v>7.6967592592592601E-5</v>
       </c>
       <c r="N32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E33" s="10">
         <v>0.2502723352076287</v>
@@ -2158,10 +2207,10 @@
         <v>0.2502723352076287</v>
       </c>
       <c r="J33" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K33" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L33" s="5">
         <f t="shared" si="7"/>
@@ -2172,21 +2221,21 @@
         <v>2.5027233520762868</v>
       </c>
       <c r="N33" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E34" s="7">
         <v>0.01</v>
@@ -2202,10 +2251,10 @@
         <v>0</v>
       </c>
       <c r="J34" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K34" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L34" s="5">
         <f t="shared" si="7"/>
@@ -2216,21 +2265,21 @@
         <v>0.1</v>
       </c>
       <c r="N34" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E35" s="7">
         <v>1.0000000000000001E-5</v>
@@ -2246,10 +2295,10 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K35" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L35" s="5">
         <f t="shared" si="7"/>
@@ -2260,21 +2309,21 @@
         <v>1E-4</v>
       </c>
       <c r="N35" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E36" s="20">
         <f>0.01/3600/24</f>
@@ -2297,10 +2346,10 @@
         <v>1.1574074074074074E-7</v>
       </c>
       <c r="J36" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K36" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L36" s="5">
         <v>0</v>
@@ -2310,20 +2359,22 @@
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N36" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="D37" s="31"/>
+        <v>63</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>88</v>
+      </c>
       <c r="E37" s="10">
         <v>0.1427507995452611</v>
       </c>
@@ -2341,10 +2392,10 @@
         <v>0.1427507995452611</v>
       </c>
       <c r="J37" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K37" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L37" s="5">
         <f t="shared" ref="L37:L44" si="10">E37/10</f>
@@ -2355,20 +2406,22 @@
         <v>1.4275079954526109</v>
       </c>
       <c r="N37" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="9"/>
+        <v>63</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>87</v>
+      </c>
       <c r="E38" s="10">
         <v>0.1427507995452611</v>
       </c>
@@ -2386,10 +2439,10 @@
         <v>0.1427507995452611</v>
       </c>
       <c r="J38" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K38" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L38" s="5">
         <f t="shared" si="10"/>
@@ -2400,20 +2453,22 @@
         <v>1.4275079954526109</v>
       </c>
       <c r="N38" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D39" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="E39" s="6">
         <v>6.4814814814814799E-17</v>
       </c>
@@ -2431,10 +2486,10 @@
         <v>0</v>
       </c>
       <c r="J39" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K39" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L39" s="5">
         <f t="shared" si="10"/>
@@ -2445,20 +2500,22 @@
         <v>6.4814814814814797E-16</v>
       </c>
       <c r="N39" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="2"/>
+        <v>64</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="E40" s="6">
         <v>4.0509259259259248E-17</v>
       </c>
@@ -2476,10 +2533,10 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K40" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L40" s="5">
         <f t="shared" si="10"/>
@@ -2490,20 +2547,22 @@
         <v>4.0509259259259247E-16</v>
       </c>
       <c r="N40" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D41" s="32"/>
+        <v>65</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>87</v>
+      </c>
       <c r="E41" s="20">
         <f>0.01/3600/24</f>
         <v>1.1574074074074074E-7</v>
@@ -2524,10 +2583,10 @@
         <v>1.1574074074074074E-7</v>
       </c>
       <c r="J41" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K41" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L41" s="5">
         <f t="shared" si="10"/>
@@ -2538,20 +2597,22 @@
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N41" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D42" s="32"/>
+        <v>65</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>88</v>
+      </c>
       <c r="E42" s="20">
         <f>0.01/3600/24</f>
         <v>1.1574074074074074E-7</v>
@@ -2572,10 +2633,10 @@
         <v>1.1574074074074074E-7</v>
       </c>
       <c r="J42" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K42" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L42" s="5">
         <f t="shared" si="10"/>
@@ -2586,20 +2647,22 @@
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N42" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="E43" s="6">
         <v>1.1574074074074101E-7</v>
       </c>
@@ -2617,10 +2680,10 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="K43" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="L43" s="5">
         <f t="shared" si="10"/>
@@ -2631,20 +2694,22 @@
         <v>1.1574074074074101E-6</v>
       </c>
       <c r="N43" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" s="19"/>
+        <v>66</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="E44" s="26">
         <v>1.1574074074074101E-7</v>
       </c>
@@ -2662,10 +2727,10 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K44" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="L44" s="5">
         <f t="shared" si="10"/>
@@ -2676,20 +2741,22 @@
         <v>1.1574074074074101E-6</v>
       </c>
       <c r="N44" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D45" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="E45" s="6">
         <v>2.083333333333333E-6</v>
       </c>
@@ -2698,23 +2765,25 @@
         <v>0.17999999999999997</v>
       </c>
       <c r="J45" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K45" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D46" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="E46" s="6">
         <v>2.083333333333333E-6</v>
       </c>
@@ -2723,58 +2792,62 @@
         <v>0.17999999999999997</v>
       </c>
       <c r="J46" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K46" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="2"/>
+        <v>68</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="E47" s="7">
         <v>0.01</v>
       </c>
       <c r="F47" s="17"/>
       <c r="J47" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K47" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D48" s="19"/>
+        <v>68</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>87</v>
+      </c>
       <c r="E48" s="20">
         <v>0.01</v>
       </c>
       <c r="F48" s="21"/>
       <c r="J48" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="K48" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J48" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:N48" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2795,7 +2868,7 @@
   <sheetData>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.25">
@@ -2803,7 +2876,7 @@
         <v>0.7</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
@@ -2812,10 +2885,10 @@
         <v>6.9999999999999993E-3</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
@@ -2824,7 +2897,7 @@
         <v>1.9444444444444444E-6</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F22">
         <f>0.4968 / (24*3600)</f>

</xml_diff>

<commit_message>
update to use 10cc as reference
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA8B715-DB69-4F45-815D-1ABD474B89AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05337041-1637-4118-B259-5BB4D74E4FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -941,7 +941,7 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,11 +1671,11 @@
       </c>
       <c r="E20" s="6">
         <f>E21/5</f>
-        <v>1.6203703703703703E-6</v>
+        <v>1.6399999999999999E-5</v>
       </c>
       <c r="F20" s="17">
         <f t="shared" si="0"/>
-        <v>0.13999999999999999</v>
+        <v>1.41696</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1690,12 +1690,12 @@
         <v>76</v>
       </c>
       <c r="L20">
-        <f t="shared" ref="L20" si="3">E20/10</f>
-        <v>1.6203703703703703E-7</v>
+        <f t="shared" ref="L20:L26" si="3">E20/10</f>
+        <v>1.64E-6</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="M20" si="4">E20*10</f>
-        <v>1.6203703703703704E-5</v>
+        <f t="shared" ref="M20:M26" si="4">E20*10</f>
+        <v>1.6399999999999997E-4</v>
       </c>
       <c r="N20" t="s">
         <v>77</v>
@@ -1715,11 +1715,11 @@
         <v>88</v>
       </c>
       <c r="E21" s="6">
-        <v>8.101851851851852E-6</v>
+        <v>8.2000000000000001E-5</v>
       </c>
       <c r="F21" s="17">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>7.0848000000000004</v>
       </c>
       <c r="J21" t="s">
         <v>77</v>
@@ -1728,12 +1728,12 @@
         <v>76</v>
       </c>
       <c r="L21">
-        <f>E21/10</f>
-        <v>8.1018518518518515E-7</v>
+        <f t="shared" si="3"/>
+        <v>8.1999999999999994E-6</v>
       </c>
       <c r="M21">
-        <f>E21*10</f>
-        <v>8.1018518518518516E-5</v>
+        <f t="shared" si="4"/>
+        <v>8.1999999999999998E-4</v>
       </c>
       <c r="N21" t="s">
         <v>77</v>
@@ -1754,11 +1754,11 @@
       </c>
       <c r="E22" s="6">
         <f>E23/5</f>
-        <v>1.1342592592592592E-5</v>
+        <v>1.2799999999999999E-5</v>
       </c>
       <c r="F22" s="17">
         <f t="shared" si="0"/>
-        <v>0.98</v>
+        <v>1.1059199999999998</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1773,12 +1773,12 @@
         <v>76</v>
       </c>
       <c r="L22">
-        <f>E22/10</f>
-        <v>1.1342592592592592E-6</v>
+        <f t="shared" si="3"/>
+        <v>1.28E-6</v>
       </c>
       <c r="M22">
-        <f>E22*10</f>
-        <v>1.1342592592592592E-4</v>
+        <f t="shared" si="4"/>
+        <v>1.2799999999999999E-4</v>
       </c>
       <c r="N22" t="s">
         <v>77</v>
@@ -1798,11 +1798,11 @@
         <v>88</v>
       </c>
       <c r="E23" s="6">
-        <v>5.6712962962962959E-5</v>
+        <v>6.3999999999999997E-5</v>
       </c>
       <c r="F23" s="17">
         <f t="shared" si="0"/>
-        <v>4.9000000000000004</v>
+        <v>5.5296000000000003</v>
       </c>
       <c r="J23" t="s">
         <v>77</v>
@@ -1811,12 +1811,12 @@
         <v>76</v>
       </c>
       <c r="L23">
-        <f t="shared" ref="L23:L26" si="5">E23/10</f>
-        <v>5.6712962962962959E-6</v>
+        <f t="shared" si="3"/>
+        <v>6.3999999999999997E-6</v>
       </c>
       <c r="M23">
-        <f t="shared" ref="M23:M26" si="6">E23*10</f>
-        <v>5.6712962962962956E-4</v>
+        <f t="shared" si="4"/>
+        <v>6.3999999999999994E-4</v>
       </c>
       <c r="N23" t="s">
         <v>77</v>
@@ -1849,11 +1849,11 @@
         <v>77</v>
       </c>
       <c r="L24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.5046296296296301E-6</v>
       </c>
       <c r="M24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.50462962962963E-4</v>
       </c>
       <c r="N24" t="s">
@@ -1887,11 +1887,11 @@
         <v>77</v>
       </c>
       <c r="L25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.5046296296296301E-6</v>
       </c>
       <c r="M25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1.50462962962963E-4</v>
       </c>
       <c r="N25" t="s">
@@ -1925,11 +1925,11 @@
         <v>77</v>
       </c>
       <c r="L26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6.7708333333333347E-6</v>
       </c>
       <c r="M26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>6.7708333333333346E-4</v>
       </c>
       <c r="N26" t="s">
@@ -2074,11 +2074,11 @@
         <v>76</v>
       </c>
       <c r="L30" s="5">
-        <f>E30/10</f>
+        <f t="shared" ref="L30:L35" si="5">E30/10</f>
         <v>6.4814814814814807E-8</v>
       </c>
       <c r="M30" s="5">
-        <f>E30*10</f>
+        <f t="shared" ref="M30:M35" si="6">E30*10</f>
         <v>6.4814814814814812E-6</v>
       </c>
       <c r="N30" t="s">
@@ -2121,11 +2121,11 @@
         <v>77</v>
       </c>
       <c r="L31" s="5">
-        <f>E31/10</f>
+        <f t="shared" si="5"/>
         <v>4.0509259259259258E-8</v>
       </c>
       <c r="M31" s="5">
-        <f>E31*10</f>
+        <f t="shared" si="6"/>
         <v>4.050925925925926E-6</v>
       </c>
       <c r="N31" t="s">
@@ -2168,11 +2168,11 @@
         <v>77</v>
       </c>
       <c r="L32" s="5">
-        <f t="shared" ref="L32:L35" si="7">E32/10</f>
+        <f t="shared" si="5"/>
         <v>7.6967592592592605E-7</v>
       </c>
       <c r="M32" s="5">
-        <f t="shared" ref="M32:M35" si="8">E32*10</f>
+        <f t="shared" si="6"/>
         <v>7.6967592592592601E-5</v>
       </c>
       <c r="N32" t="s">
@@ -2215,11 +2215,11 @@
         <v>77</v>
       </c>
       <c r="L33" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>2.502723352076287E-2</v>
       </c>
       <c r="M33" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>2.5027233520762868</v>
       </c>
       <c r="N33" t="s">
@@ -2259,11 +2259,11 @@
         <v>76</v>
       </c>
       <c r="L34" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1E-3</v>
       </c>
       <c r="M34" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
       <c r="N34" t="s">
@@ -2303,11 +2303,11 @@
         <v>77</v>
       </c>
       <c r="L35" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000002E-6</v>
       </c>
       <c r="M35" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1E-4</v>
       </c>
       <c r="N35" t="s">
@@ -2357,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="5">
-        <f t="shared" ref="M36:M44" si="9">E36*10</f>
+        <f t="shared" ref="M36:M44" si="7">E36*10</f>
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N36" t="s">
@@ -2400,11 +2400,11 @@
         <v>76</v>
       </c>
       <c r="L37" s="5">
-        <f t="shared" ref="L37:L44" si="10">E37/10</f>
+        <f t="shared" ref="L37:L44" si="8">E37/10</f>
         <v>1.427507995452611E-2</v>
       </c>
       <c r="M37" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.4275079954526109</v>
       </c>
       <c r="N37" t="s">
@@ -2447,11 +2447,11 @@
         <v>77</v>
       </c>
       <c r="L38" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1.427507995452611E-2</v>
       </c>
       <c r="M38" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.4275079954526109</v>
       </c>
       <c r="N38" t="s">
@@ -2494,11 +2494,11 @@
         <v>76</v>
       </c>
       <c r="L39" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>6.4814814814814798E-18</v>
       </c>
       <c r="M39" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>6.4814814814814797E-16</v>
       </c>
       <c r="N39" t="s">
@@ -2541,11 +2541,11 @@
         <v>77</v>
       </c>
       <c r="L40" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>4.050925925925925E-18</v>
       </c>
       <c r="M40" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>4.0509259259259247E-16</v>
       </c>
       <c r="N40" t="s">
@@ -2591,11 +2591,11 @@
         <v>77</v>
       </c>
       <c r="L41" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1.1574074074074074E-8</v>
       </c>
       <c r="M41" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N41" t="s">
@@ -2641,11 +2641,11 @@
         <v>76</v>
       </c>
       <c r="L42" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1.1574074074074074E-8</v>
       </c>
       <c r="M42" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N42" t="s">
@@ -2688,11 +2688,11 @@
         <v>76</v>
       </c>
       <c r="L43" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1.15740740740741E-8</v>
       </c>
       <c r="M43" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.1574074074074101E-6</v>
       </c>
       <c r="N43" t="s">
@@ -2735,11 +2735,11 @@
         <v>77</v>
       </c>
       <c r="L44" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>1.15740740740741E-8</v>
       </c>
       <c r="M44" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.1574074074074101E-6</v>
       </c>
       <c r="N44" t="s">

</xml_diff>

<commit_message>
change bound to /5  - *5
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B705671A-F6DE-4D12-899F-8B5BF1AD36E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF06FEE0-8C94-45F0-82BD-388D6A675537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="107">
   <si>
     <t>Mh</t>
   </si>
@@ -352,6 +352,12 @@
   </si>
   <si>
     <t>VmaxROSh</t>
+  </si>
+  <si>
+    <t>lower bound orig</t>
+  </si>
+  <si>
+    <t>upper bound orig</t>
   </si>
 </sst>
 </file>
@@ -938,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +965,7 @@
     <col min="12" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="29" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="29" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>46</v>
       </c>
@@ -1002,8 +1008,14 @@
       <c r="N1" s="29" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -1030,8 +1042,8 @@
         <v>77</v>
       </c>
       <c r="L2" s="5">
-        <f>E2/10</f>
-        <v>1.157407407407407E-7</v>
+        <f>E2/5</f>
+        <v>2.314814814814814E-7</v>
       </c>
       <c r="M2" s="5">
         <f>E2*100</f>
@@ -1040,8 +1052,14 @@
       <c r="N2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>1.157407407407407E-7</v>
+      </c>
+      <c r="P2">
+        <v>1.1574074074074069E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -1068,18 +1086,24 @@
         <v>76</v>
       </c>
       <c r="L3" s="5">
-        <f>E3/10</f>
+        <f>E3/5</f>
+        <v>2.314814814814814E-7</v>
+      </c>
+      <c r="M3" s="5">
+        <f>E3*5</f>
+        <v>5.7870370370370351E-6</v>
+      </c>
+      <c r="N3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O3">
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="M3" s="5">
-        <f>E3*100</f>
+      <c r="P3">
         <v>1.1574074074074069E-4</v>
       </c>
-      <c r="N3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -1111,8 +1135,14 @@
       <c r="N4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O4">
+        <v>0.1</v>
+      </c>
+      <c r="P4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>3</v>
       </c>
@@ -1144,8 +1174,14 @@
       <c r="N5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>0.1</v>
+      </c>
+      <c r="P5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
@@ -1169,7 +1205,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>5</v>
       </c>
@@ -1193,7 +1229,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
@@ -1223,18 +1259,24 @@
         <v>76</v>
       </c>
       <c r="L8" s="5">
-        <f>E8/10</f>
+        <f>E8/5</f>
+        <v>2.314814814814814E-7</v>
+      </c>
+      <c r="M8" s="5">
+        <f>E8*5</f>
+        <v>5.7870370370370351E-6</v>
+      </c>
+      <c r="N8" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8">
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="M8" s="5">
-        <f>E8*10</f>
+      <c r="P8">
         <v>1.157407407407407E-5</v>
       </c>
-      <c r="N8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -1270,7 +1312,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -1300,18 +1342,24 @@
         <v>77</v>
       </c>
       <c r="L10" s="5">
-        <f>E10/10</f>
+        <f>E10/5</f>
+        <v>2.314814814814814E-7</v>
+      </c>
+      <c r="M10" s="5">
+        <f>E10*5</f>
+        <v>5.7870370370370351E-6</v>
+      </c>
+      <c r="N10" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10">
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="M10" s="5">
-        <f>E10*10</f>
+      <c r="P10">
         <v>1.157407407407407E-5</v>
       </c>
-      <c r="N10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>9</v>
       </c>
@@ -1347,7 +1395,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
@@ -1380,18 +1428,24 @@
         <v>76</v>
       </c>
       <c r="L12">
-        <f>E12/10</f>
+        <f>E12/5</f>
+        <v>2.8550159909052221E-2</v>
+      </c>
+      <c r="M12">
+        <f>E12*5</f>
+        <v>0.71375399772630543</v>
+      </c>
+      <c r="N12" t="s">
+        <v>77</v>
+      </c>
+      <c r="O12">
         <v>1.427507995452611E-2</v>
       </c>
-      <c r="M12">
-        <f>E12*10</f>
+      <c r="P12">
         <v>1.4275079954526109</v>
       </c>
-      <c r="N12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -1415,18 +1469,24 @@
         <v>76</v>
       </c>
       <c r="L13">
-        <f t="shared" ref="L13:L19" si="1">E13/10</f>
+        <f t="shared" ref="L13:L26" si="1">E13/5</f>
+        <v>2.8550159909052221E-2</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ref="M13:M26" si="2">E13*5</f>
+        <v>0.71375399772630543</v>
+      </c>
+      <c r="N13" t="s">
+        <v>77</v>
+      </c>
+      <c r="O13">
         <v>1.427507995452611E-2</v>
       </c>
-      <c r="M13">
-        <f t="shared" ref="M13:M19" si="2">E13*10</f>
+      <c r="P13">
         <v>1.4275079954526109</v>
       </c>
-      <c r="N13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -1459,17 +1519,23 @@
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
-        <v>1.427507995452611E-2</v>
+        <v>2.8550159909052221E-2</v>
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
+        <v>0.71375399772630543</v>
+      </c>
+      <c r="N14" t="s">
+        <v>77</v>
+      </c>
+      <c r="O14">
+        <v>1.427507995452611E-2</v>
+      </c>
+      <c r="P14">
         <v>1.4275079954526109</v>
       </c>
-      <c r="N14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
@@ -1494,17 +1560,23 @@
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
-        <v>1.427507995452611E-2</v>
+        <v>2.8550159909052221E-2</v>
       </c>
       <c r="M15">
         <f t="shared" si="2"/>
+        <v>0.71375399772630543</v>
+      </c>
+      <c r="N15" t="s">
+        <v>77</v>
+      </c>
+      <c r="O15">
+        <v>1.427507995452611E-2</v>
+      </c>
+      <c r="P15">
         <v>1.4275079954526109</v>
       </c>
-      <c r="N15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
@@ -1529,17 +1601,23 @@
       </c>
       <c r="L16">
         <f t="shared" si="1"/>
-        <v>2.502723352076287E-2</v>
+        <v>5.005446704152574E-2</v>
       </c>
       <c r="M16">
         <f t="shared" si="2"/>
+        <v>1.2513616760381434</v>
+      </c>
+      <c r="N16" t="s">
+        <v>77</v>
+      </c>
+      <c r="O16">
+        <v>2.502723352076287E-2</v>
+      </c>
+      <c r="P16">
         <v>2.5027233520762868</v>
       </c>
-      <c r="N16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -1564,17 +1642,23 @@
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
-        <v>2.502723352076287E-2</v>
+        <v>5.005446704152574E-2</v>
       </c>
       <c r="M17">
         <f t="shared" si="2"/>
+        <v>1.2513616760381434</v>
+      </c>
+      <c r="N17" t="s">
+        <v>77</v>
+      </c>
+      <c r="O17">
+        <v>2.502723352076287E-2</v>
+      </c>
+      <c r="P17">
         <v>2.5027233520762868</v>
       </c>
-      <c r="N17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>16</v>
       </c>
@@ -1599,17 +1683,23 @@
       </c>
       <c r="L18">
         <f t="shared" si="1"/>
-        <v>2.502723352076287E-2</v>
+        <v>5.005446704152574E-2</v>
       </c>
       <c r="M18">
         <f t="shared" si="2"/>
+        <v>1.2513616760381434</v>
+      </c>
+      <c r="N18" t="s">
+        <v>77</v>
+      </c>
+      <c r="O18">
+        <v>2.502723352076287E-2</v>
+      </c>
+      <c r="P18">
         <v>2.5027233520762868</v>
       </c>
-      <c r="N18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>17</v>
       </c>
@@ -1646,17 +1736,23 @@
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
-        <v>2.502723352076287E-2</v>
+        <v>5.005446704152574E-2</v>
       </c>
       <c r="M19">
         <f t="shared" si="2"/>
+        <v>1.2513616760381434</v>
+      </c>
+      <c r="N19" t="s">
+        <v>77</v>
+      </c>
+      <c r="O19">
+        <v>2.502723352076287E-2</v>
+      </c>
+      <c r="P19">
         <v>2.5027233520762868</v>
       </c>
-      <c r="N19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>18</v>
       </c>
@@ -1690,18 +1786,24 @@
         <v>76</v>
       </c>
       <c r="L20">
-        <f t="shared" ref="L20:L26" si="3">E20/10</f>
+        <f t="shared" si="1"/>
+        <v>3.2799999999999999E-6</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="2"/>
+        <v>8.1999999999999987E-5</v>
+      </c>
+      <c r="N20" t="s">
+        <v>77</v>
+      </c>
+      <c r="O20">
         <v>1.64E-6</v>
       </c>
-      <c r="M20">
-        <f t="shared" ref="M20:M26" si="4">E20*10</f>
+      <c r="P20">
         <v>1.6399999999999997E-4</v>
       </c>
-      <c r="N20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>19</v>
       </c>
@@ -1728,18 +1830,24 @@
         <v>76</v>
       </c>
       <c r="L21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
+        <v>1.6399999999999999E-5</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="2"/>
+        <v>4.0999999999999999E-4</v>
+      </c>
+      <c r="N21" t="s">
+        <v>77</v>
+      </c>
+      <c r="O21">
         <v>8.1999999999999994E-6</v>
       </c>
-      <c r="M21">
-        <f t="shared" si="4"/>
+      <c r="P21">
         <v>8.1999999999999998E-4</v>
       </c>
-      <c r="N21" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>20</v>
       </c>
@@ -1773,18 +1881,24 @@
         <v>76</v>
       </c>
       <c r="L22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
+        <v>2.5600000000000001E-6</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="2"/>
+        <v>6.3999999999999997E-5</v>
+      </c>
+      <c r="N22" t="s">
+        <v>77</v>
+      </c>
+      <c r="O22">
         <v>1.28E-6</v>
       </c>
-      <c r="M22">
-        <f t="shared" si="4"/>
+      <c r="P22">
         <v>1.2799999999999999E-4</v>
       </c>
-      <c r="N22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>21</v>
       </c>
@@ -1811,18 +1925,24 @@
         <v>76</v>
       </c>
       <c r="L23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
+        <v>1.2799999999999999E-5</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="2"/>
+        <v>3.1999999999999997E-4</v>
+      </c>
+      <c r="N23" t="s">
+        <v>77</v>
+      </c>
+      <c r="O23">
         <v>6.3999999999999997E-6</v>
       </c>
-      <c r="M23">
-        <f t="shared" si="4"/>
+      <c r="P23">
         <v>6.3999999999999994E-4</v>
       </c>
-      <c r="N23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>22</v>
       </c>
@@ -1849,18 +1969,24 @@
         <v>77</v>
       </c>
       <c r="L24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
+        <v>3.0092592592592601E-6</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="2"/>
+        <v>7.5231481481481501E-5</v>
+      </c>
+      <c r="N24" t="s">
+        <v>77</v>
+      </c>
+      <c r="O24">
         <v>1.5046296296296301E-6</v>
       </c>
-      <c r="M24">
-        <f t="shared" si="4"/>
+      <c r="P24">
         <v>1.50462962962963E-4</v>
       </c>
-      <c r="N24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>23</v>
       </c>
@@ -1887,18 +2013,24 @@
         <v>77</v>
       </c>
       <c r="L25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
+        <v>3.0092592592592601E-6</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="2"/>
+        <v>7.5231481481481501E-5</v>
+      </c>
+      <c r="N25" t="s">
+        <v>77</v>
+      </c>
+      <c r="O25">
         <v>1.5046296296296301E-6</v>
       </c>
-      <c r="M25">
-        <f t="shared" si="4"/>
+      <c r="P25">
         <v>1.50462962962963E-4</v>
       </c>
-      <c r="N25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>24</v>
       </c>
@@ -1925,18 +2057,24 @@
         <v>77</v>
       </c>
       <c r="L26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
+        <v>1.3541666666666669E-5</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="2"/>
+        <v>3.3854166666666673E-4</v>
+      </c>
+      <c r="N26" t="s">
+        <v>77</v>
+      </c>
+      <c r="O26">
         <v>6.7708333333333347E-6</v>
       </c>
-      <c r="M26">
-        <f t="shared" si="4"/>
+      <c r="P26">
         <v>6.7708333333333346E-4</v>
       </c>
-      <c r="N26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>25</v>
       </c>
@@ -1972,7 +2110,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>26</v>
       </c>
@@ -2005,7 +2143,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>27</v>
       </c>
@@ -2038,7 +2176,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>28</v>
       </c>
@@ -2074,18 +2212,24 @@
         <v>76</v>
       </c>
       <c r="L30" s="5">
-        <f t="shared" ref="L30:L35" si="5">E30/10</f>
+        <f t="shared" ref="L30:L35" si="3">E30/10</f>
         <v>6.4814814814814807E-8</v>
       </c>
       <c r="M30" s="5">
-        <f t="shared" ref="M30:M35" si="6">E30*10</f>
+        <f t="shared" ref="M30:M35" si="4">E30*10</f>
         <v>6.4814814814814812E-6</v>
       </c>
       <c r="N30" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <v>6.4814814814814807E-8</v>
+      </c>
+      <c r="P30">
+        <v>6.4814814814814812E-6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>29</v>
       </c>
@@ -2121,18 +2265,24 @@
         <v>77</v>
       </c>
       <c r="L31" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4.0509259259259258E-8</v>
       </c>
       <c r="M31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>4.050925925925926E-6</v>
       </c>
       <c r="N31" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <v>4.0509259259259258E-8</v>
+      </c>
+      <c r="P31">
+        <v>4.050925925925926E-6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>104</v>
       </c>
@@ -2168,18 +2318,24 @@
         <v>77</v>
       </c>
       <c r="L32" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>7.6967592592592605E-7</v>
       </c>
       <c r="M32" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>7.6967592592592601E-5</v>
       </c>
       <c r="N32" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <v>7.6967592592592605E-7</v>
+      </c>
+      <c r="P32">
+        <v>7.6967592592592601E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>30</v>
       </c>
@@ -2215,18 +2371,24 @@
         <v>77</v>
       </c>
       <c r="L33" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>2.502723352076287E-2</v>
       </c>
       <c r="M33" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>2.5027233520762868</v>
       </c>
       <c r="N33" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <v>2.502723352076287E-2</v>
+      </c>
+      <c r="P33">
+        <v>2.5027233520762868</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>31</v>
       </c>
@@ -2259,18 +2421,24 @@
         <v>76</v>
       </c>
       <c r="L34" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1E-3</v>
       </c>
       <c r="M34" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="N34" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <v>1E-3</v>
+      </c>
+      <c r="P34">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>32</v>
       </c>
@@ -2303,18 +2471,24 @@
         <v>77</v>
       </c>
       <c r="L35" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1.0000000000000002E-6</v>
       </c>
       <c r="M35" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>1E-4</v>
       </c>
       <c r="N35" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O35">
+        <v>1.0000000000000002E-6</v>
+      </c>
+      <c r="P35">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
         <v>33</v>
       </c>
@@ -2357,14 +2531,20 @@
         <v>0</v>
       </c>
       <c r="M36" s="5">
-        <f t="shared" ref="M36:M44" si="7">E36*10</f>
+        <f t="shared" ref="M36:M44" si="5">E36*10</f>
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N36" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>1.1574074074074074E-6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>34</v>
       </c>
@@ -2400,18 +2580,24 @@
         <v>76</v>
       </c>
       <c r="L37" s="5">
-        <f t="shared" ref="L37:L44" si="8">E37/10</f>
+        <f t="shared" ref="L37:L44" si="6">E37/10</f>
         <v>1.427507995452611E-2</v>
       </c>
       <c r="M37" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.4275079954526109</v>
       </c>
       <c r="N37" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <v>1.427507995452611E-2</v>
+      </c>
+      <c r="P37">
+        <v>1.4275079954526109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>35</v>
       </c>
@@ -2447,18 +2633,24 @@
         <v>77</v>
       </c>
       <c r="L38" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.427507995452611E-2</v>
       </c>
       <c r="M38" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.4275079954526109</v>
       </c>
       <c r="N38" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <v>1.427507995452611E-2</v>
+      </c>
+      <c r="P38">
+        <v>1.4275079954526109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>36</v>
       </c>
@@ -2494,18 +2686,24 @@
         <v>76</v>
       </c>
       <c r="L39" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>6.4814814814814798E-18</v>
       </c>
       <c r="M39" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>6.4814814814814797E-16</v>
       </c>
       <c r="N39" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <v>6.4814814814814798E-18</v>
+      </c>
+      <c r="P39">
+        <v>6.4814814814814797E-16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>37</v>
       </c>
@@ -2541,18 +2739,24 @@
         <v>77</v>
       </c>
       <c r="L40" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>4.050925925925925E-18</v>
       </c>
       <c r="M40" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>4.0509259259259247E-16</v>
       </c>
       <c r="N40" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O40">
+        <v>4.050925925925925E-18</v>
+      </c>
+      <c r="P40">
+        <v>4.0509259259259247E-16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
         <v>38</v>
       </c>
@@ -2591,18 +2795,24 @@
         <v>77</v>
       </c>
       <c r="L41" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.1574074074074074E-8</v>
       </c>
       <c r="M41" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N41" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O41">
+        <v>1.1574074074074074E-8</v>
+      </c>
+      <c r="P41">
+        <v>1.1574074074074074E-6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
         <v>39</v>
       </c>
@@ -2641,18 +2851,24 @@
         <v>76</v>
       </c>
       <c r="L42" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.1574074074074074E-8</v>
       </c>
       <c r="M42" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N42" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <v>1.1574074074074074E-8</v>
+      </c>
+      <c r="P42">
+        <v>1.1574074074074074E-6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>40</v>
       </c>
@@ -2688,18 +2904,24 @@
         <v>76</v>
       </c>
       <c r="L43" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.15740740740741E-8</v>
       </c>
       <c r="M43" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.1574074074074101E-6</v>
       </c>
       <c r="N43" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O43">
+        <v>1.15740740740741E-8</v>
+      </c>
+      <c r="P43">
+        <v>1.1574074074074101E-6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18" t="s">
         <v>41</v>
       </c>
@@ -2735,18 +2957,24 @@
         <v>77</v>
       </c>
       <c r="L44" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>1.15740740740741E-8</v>
       </c>
       <c r="M44" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.1574074074074101E-6</v>
       </c>
       <c r="N44" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <v>1.15740740740741E-8</v>
+      </c>
+      <c r="P44">
+        <v>1.1574074074074101E-6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>42</v>
       </c>
@@ -2773,7 +3001,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>43</v>
       </c>
@@ -2800,7 +3028,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>44</v>
       </c>
@@ -2824,7 +3052,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
debug least square het
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF06FEE0-8C94-45F0-82BD-388D6A675537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260C3B0B-8DDA-4878-86F5-123AFD91AB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,12 +387,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -568,7 +574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -640,6 +646,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -947,7 +962,7 @@
   <dimension ref="A1:P48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,12 +1057,12 @@
         <v>77</v>
       </c>
       <c r="L2" s="5">
-        <f>E2/5</f>
-        <v>2.314814814814814E-7</v>
+        <f>E2/10</f>
+        <v>1.157407407407407E-7</v>
       </c>
       <c r="M2" s="5">
-        <f>E2*100</f>
-        <v>1.1574074074074069E-4</v>
+        <f>E2*10</f>
+        <v>1.157407407407407E-5</v>
       </c>
       <c r="N2" t="s">
         <v>77</v>
@@ -1206,28 +1221,36 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="35">
         <v>4.5</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="J7" t="s">
-        <v>76</v>
-      </c>
-      <c r="K7" t="s">
-        <v>77</v>
-      </c>
+      <c r="F7" s="36"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
@@ -1342,12 +1365,12 @@
         <v>77</v>
       </c>
       <c r="L10" s="5">
-        <f>E10/5</f>
-        <v>2.314814814814814E-7</v>
+        <f>E10/10</f>
+        <v>1.157407407407407E-7</v>
       </c>
       <c r="M10" s="5">
-        <f>E10*5</f>
-        <v>5.7870370370370351E-6</v>
+        <f>E10*10</f>
+        <v>1.157407407407407E-5</v>
       </c>
       <c r="N10" t="s">
         <v>77</v>
@@ -1599,16 +1622,16 @@
       <c r="K16" t="s">
         <v>77</v>
       </c>
-      <c r="L16">
-        <f t="shared" si="1"/>
-        <v>5.005446704152574E-2</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="2"/>
+      <c r="L16" s="5">
+        <f t="shared" ref="L16:L18" si="3">E16/10</f>
+        <v>2.502723352076287E-2</v>
+      </c>
+      <c r="M16" s="5">
+        <f>E16*5</f>
         <v>1.2513616760381434</v>
       </c>
       <c r="N16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O16">
         <v>2.502723352076287E-2</v>
@@ -1640,16 +1663,16 @@
       <c r="K17" t="s">
         <v>77</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="1"/>
-        <v>5.005446704152574E-2</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="2"/>
+      <c r="L17" s="5">
+        <f t="shared" si="3"/>
+        <v>2.502723352076287E-2</v>
+      </c>
+      <c r="M17" s="5">
+        <f t="shared" ref="M17:M18" si="4">E17*5</f>
         <v>1.2513616760381434</v>
       </c>
       <c r="N17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O17">
         <v>2.502723352076287E-2</v>
@@ -1681,16 +1704,16 @@
       <c r="K18" t="s">
         <v>77</v>
       </c>
-      <c r="L18">
-        <f t="shared" si="1"/>
-        <v>5.005446704152574E-2</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="2"/>
+      <c r="L18" s="5">
+        <f t="shared" si="3"/>
+        <v>2.502723352076287E-2</v>
+      </c>
+      <c r="M18" s="5">
+        <f t="shared" si="4"/>
         <v>1.2513616760381434</v>
       </c>
       <c r="N18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O18">
         <v>2.502723352076287E-2</v>
@@ -1968,13 +1991,13 @@
       <c r="K24" t="s">
         <v>77</v>
       </c>
-      <c r="L24">
-        <f t="shared" si="1"/>
-        <v>3.0092592592592601E-6</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="2"/>
-        <v>7.5231481481481501E-5</v>
+      <c r="L24" s="5">
+        <f t="shared" ref="L24:L26" si="5">E24/10</f>
+        <v>1.5046296296296301E-6</v>
+      </c>
+      <c r="M24" s="5">
+        <f t="shared" ref="M24:M26" si="6">E24*10</f>
+        <v>1.50462962962963E-4</v>
       </c>
       <c r="N24" t="s">
         <v>77</v>
@@ -2012,13 +2035,13 @@
       <c r="K25" t="s">
         <v>77</v>
       </c>
-      <c r="L25">
-        <f t="shared" si="1"/>
-        <v>3.0092592592592601E-6</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="2"/>
-        <v>7.5231481481481501E-5</v>
+      <c r="L25" s="5">
+        <f t="shared" si="5"/>
+        <v>1.5046296296296301E-6</v>
+      </c>
+      <c r="M25" s="5">
+        <f t="shared" si="6"/>
+        <v>1.50462962962963E-4</v>
       </c>
       <c r="N25" t="s">
         <v>77</v>
@@ -2056,13 +2079,13 @@
       <c r="K26" t="s">
         <v>77</v>
       </c>
-      <c r="L26">
-        <f t="shared" si="1"/>
-        <v>1.3541666666666669E-5</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="2"/>
-        <v>3.3854166666666673E-4</v>
+      <c r="L26" s="5">
+        <f t="shared" si="5"/>
+        <v>6.7708333333333347E-6</v>
+      </c>
+      <c r="M26" s="5">
+        <f t="shared" si="6"/>
+        <v>6.7708333333333346E-4</v>
       </c>
       <c r="N26" t="s">
         <v>77</v>
@@ -2212,11 +2235,11 @@
         <v>76</v>
       </c>
       <c r="L30" s="5">
-        <f t="shared" ref="L30:L35" si="3">E30/10</f>
+        <f t="shared" ref="L30:L35" si="7">E30/10</f>
         <v>6.4814814814814807E-8</v>
       </c>
       <c r="M30" s="5">
-        <f t="shared" ref="M30:M35" si="4">E30*10</f>
+        <f t="shared" ref="M30:M35" si="8">E30*10</f>
         <v>6.4814814814814812E-6</v>
       </c>
       <c r="N30" t="s">
@@ -2265,11 +2288,11 @@
         <v>77</v>
       </c>
       <c r="L31" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4.0509259259259258E-8</v>
       </c>
       <c r="M31" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4.050925925925926E-6</v>
       </c>
       <c r="N31" t="s">
@@ -2318,11 +2341,11 @@
         <v>77</v>
       </c>
       <c r="L32" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>7.6967592592592605E-7</v>
       </c>
       <c r="M32" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>7.6967592592592601E-5</v>
       </c>
       <c r="N32" t="s">
@@ -2371,12 +2394,12 @@
         <v>77</v>
       </c>
       <c r="L33" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2.502723352076287E-2</v>
       </c>
       <c r="M33" s="5">
-        <f t="shared" si="4"/>
-        <v>2.5027233520762868</v>
+        <f>E33*5</f>
+        <v>1.2513616760381434</v>
       </c>
       <c r="N33" t="s">
         <v>77</v>
@@ -2421,11 +2444,11 @@
         <v>76</v>
       </c>
       <c r="L34" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1E-3</v>
       </c>
       <c r="M34" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.1</v>
       </c>
       <c r="N34" t="s">
@@ -2471,11 +2494,11 @@
         <v>77</v>
       </c>
       <c r="L35" s="5">
-        <f t="shared" si="3"/>
+        <f>E35/10</f>
         <v>1.0000000000000002E-6</v>
       </c>
       <c r="M35" s="5">
-        <f t="shared" si="4"/>
+        <f>E35*10</f>
         <v>1E-4</v>
       </c>
       <c r="N35" t="s">
@@ -2531,7 +2554,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="5">
-        <f t="shared" ref="M36:M44" si="5">E36*10</f>
+        <f t="shared" ref="M36:M44" si="9">E36*10</f>
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N36" t="s">
@@ -2580,11 +2603,11 @@
         <v>76</v>
       </c>
       <c r="L37" s="5">
-        <f t="shared" ref="L37:L44" si="6">E37/10</f>
+        <f t="shared" ref="L37:L44" si="10">E37/10</f>
         <v>1.427507995452611E-2</v>
       </c>
       <c r="M37" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.4275079954526109</v>
       </c>
       <c r="N37" t="s">
@@ -2633,11 +2656,11 @@
         <v>77</v>
       </c>
       <c r="L38" s="5">
-        <f t="shared" si="6"/>
+        <f>E38/10</f>
         <v>1.427507995452611E-2</v>
       </c>
       <c r="M38" s="5">
-        <f t="shared" si="5"/>
+        <f>E38*10</f>
         <v>1.4275079954526109</v>
       </c>
       <c r="N38" t="s">
@@ -2686,11 +2709,11 @@
         <v>76</v>
       </c>
       <c r="L39" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>6.4814814814814798E-18</v>
       </c>
       <c r="M39" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6.4814814814814797E-16</v>
       </c>
       <c r="N39" t="s">
@@ -2739,11 +2762,11 @@
         <v>77</v>
       </c>
       <c r="L40" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.050925925925925E-18</v>
       </c>
       <c r="M40" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.0509259259259247E-16</v>
       </c>
       <c r="N40" t="s">
@@ -2795,11 +2818,11 @@
         <v>77</v>
       </c>
       <c r="L41" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.1574074074074074E-8</v>
       </c>
       <c r="M41" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N41" t="s">
@@ -2851,11 +2874,11 @@
         <v>76</v>
       </c>
       <c r="L42" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.1574074074074074E-8</v>
       </c>
       <c r="M42" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.1574074074074074E-6</v>
       </c>
       <c r="N42" t="s">
@@ -2904,11 +2927,11 @@
         <v>76</v>
       </c>
       <c r="L43" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1.15740740740741E-8</v>
       </c>
       <c r="M43" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.1574074074074101E-6</v>
       </c>
       <c r="N43" t="s">
@@ -2957,11 +2980,11 @@
         <v>77</v>
       </c>
       <c r="L44" s="5">
-        <f t="shared" si="6"/>
+        <f>E44/10</f>
         <v>1.15740740740741E-8</v>
       </c>
       <c r="M44" s="5">
-        <f t="shared" si="5"/>
+        <f>E44*10</f>
         <v>1.1574074074074101E-6</v>
       </c>
       <c r="N44" t="s">

</xml_diff>

<commit_message>
bug fix store model
</commit_message>
<xml_diff>
--- a/Model_Parameters.xlsx
+++ b/Model_Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB71E8D-E4B0-4900-AACF-80393B2F562D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE568FF-2EFC-428B-8E35-51D9E9FEE922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,7 +458,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -479,19 +479,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -614,24 +601,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -642,8 +616,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -653,65 +625,54 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,8 +979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,111 +998,117 @@
     <col min="15" max="17" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="29" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:19" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="29" t="s">
+      <c r="Q1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="R1" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="S1" s="29" t="s">
+      <c r="S1" s="23" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="4">
         <v>1.157407407407407E-6</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="5">
         <f>E2*3600*24</f>
         <v>9.999999999999995E-2</v>
       </c>
-      <c r="M2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N2" t="s">
-        <v>73</v>
-      </c>
-      <c r="O2" s="5">
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" s="4">
         <f>E2/10</f>
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="P2" s="5">
+      <c r="P2" s="4">
         <f>E2*10</f>
         <v>1.157407407407407E-5</v>
       </c>
-      <c r="Q2" t="s">
-        <v>73</v>
-      </c>
-      <c r="R2">
+      <c r="Q2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R2" s="5">
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="10">
         <v>1.1574074074074069E-4</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1153,39 +1120,45 @@
       <c r="D3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>1.157407407407407E-6</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="5">
         <f t="shared" ref="F3:F48" si="0">E3*3600*24</f>
         <v>9.999999999999995E-2</v>
       </c>
-      <c r="M3" t="s">
-        <v>73</v>
-      </c>
-      <c r="N3" t="s">
-        <v>72</v>
-      </c>
-      <c r="O3" s="5">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" s="4">
         <f>E3/5</f>
         <v>2.314814814814814E-7</v>
       </c>
-      <c r="P3" s="5">
+      <c r="P3" s="4">
         <f>E3*5</f>
         <v>5.7870370370370351E-6</v>
       </c>
-      <c r="Q3" t="s">
-        <v>73</v>
-      </c>
-      <c r="R3">
+      <c r="Q3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R3" s="5">
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="10">
         <v>1.1574074074074069E-4</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1197,176 +1170,205 @@
       <c r="D4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>0.6</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="M4" t="s">
-        <v>73</v>
-      </c>
-      <c r="N4" t="s">
-        <v>72</v>
-      </c>
-      <c r="O4">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O4" s="5">
         <v>0.1</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="5">
         <v>0.9</v>
       </c>
-      <c r="Q4" t="s">
-        <v>72</v>
-      </c>
-      <c r="R4">
+      <c r="Q4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="5">
         <v>0.1</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="10">
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="5">
         <v>0.6</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="M5" t="s">
-        <v>72</v>
-      </c>
-      <c r="N5" t="s">
-        <v>73</v>
-      </c>
-      <c r="O5">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O5" s="5">
         <v>0.1</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="5">
         <v>0.9</v>
       </c>
-      <c r="Q5" t="s">
-        <v>72</v>
-      </c>
-      <c r="R5">
+      <c r="Q5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R5" s="5">
         <v>0.1</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="10">
         <v>0.9</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="5">
         <v>7</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="M6" t="s">
-        <v>72</v>
-      </c>
-      <c r="N6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="10"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="17">
         <v>4.5</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="N7" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="25"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="4">
         <v>1.157407407407407E-6</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>9.999999999999995E-2</v>
       </c>
-      <c r="M8" t="s">
-        <v>73</v>
-      </c>
-      <c r="N8" t="s">
-        <v>72</v>
-      </c>
-      <c r="O8" s="5">
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O8" s="4">
         <f>E8/5</f>
         <v>2.314814814814814E-7</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="4">
         <f>E8*5</f>
         <v>5.7870370370370351E-6</v>
       </c>
-      <c r="Q8" t="s">
-        <v>73</v>
-      </c>
-      <c r="R8">
+      <c r="Q8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R8" s="5">
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="10">
         <v>1.157407407407407E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1378,978 +1380,1091 @@
       <c r="D9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="7">
-        <v>0</v>
-      </c>
-      <c r="F9" s="17">
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M9" t="s">
-        <v>72</v>
-      </c>
-      <c r="N9" t="s">
-        <v>72</v>
-      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="10"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="4">
         <v>1.157407407407407E-6</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="5">
         <f t="shared" si="0"/>
         <v>9.999999999999995E-2</v>
       </c>
-      <c r="M10" t="s">
-        <v>72</v>
-      </c>
-      <c r="N10" t="s">
-        <v>73</v>
-      </c>
-      <c r="O10" s="5">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O10" s="4">
         <f>E10/10</f>
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="P10" s="5">
+      <c r="P10" s="4">
         <f>E10*10</f>
         <v>1.157407407407407E-5</v>
       </c>
-      <c r="Q10" t="s">
-        <v>73</v>
-      </c>
-      <c r="R10">
+      <c r="Q10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R10" s="5">
         <v>1.157407407407407E-7</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="10">
         <v>1.157407407407407E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="20">
-        <v>0</v>
-      </c>
-      <c r="F11" s="21">
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M11" t="s">
-        <v>72</v>
-      </c>
-      <c r="N11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="10"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="8">
         <v>0.1427507995452611</v>
       </c>
-      <c r="F12" s="15"/>
-      <c r="G12" s="4">
+      <c r="F12" s="5"/>
+      <c r="G12" s="8">
         <f>$E12</f>
         <v>0.1427507995452611</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="8">
         <f t="shared" ref="H12:K12" si="1">$E12</f>
         <v>0.1427507995452611</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="8">
         <f t="shared" si="1"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="8">
         <f t="shared" si="1"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="8">
         <f t="shared" si="1"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" t="s">
-        <v>73</v>
-      </c>
-      <c r="N12" t="s">
-        <v>72</v>
-      </c>
-      <c r="O12">
+      <c r="L12" s="8"/>
+      <c r="M12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" s="5">
         <f>E12/5</f>
         <v>2.8550159909052221E-2</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="5">
         <f>E12*5</f>
         <v>0.71375399772630543</v>
       </c>
-      <c r="Q12" t="s">
-        <v>73</v>
-      </c>
-      <c r="R12">
+      <c r="Q12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R12" s="5">
         <v>1.427507995452611E-2</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="10">
         <v>1.4275079954526109</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="8">
         <v>0.1427507995452611</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="M13" t="s">
-        <v>73</v>
-      </c>
-      <c r="N13" t="s">
-        <v>72</v>
-      </c>
-      <c r="O13">
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O13" s="5">
         <f t="shared" ref="O13:O23" si="2">E13/5</f>
         <v>2.8550159909052221E-2</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="5">
         <f t="shared" ref="P13:P23" si="3">E13*5</f>
         <v>0.71375399772630543</v>
       </c>
-      <c r="Q13" t="s">
-        <v>73</v>
-      </c>
-      <c r="R13">
+      <c r="Q13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R13" s="5">
         <v>1.427507995452611E-2</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="10">
         <v>1.4275079954526109</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="8">
         <v>0.1427507995452611</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="4">
+      <c r="F14" s="5"/>
+      <c r="G14" s="8">
         <f>$E14</f>
         <v>0.1427507995452611</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="8">
         <f t="shared" ref="H14:K14" si="4">$E14</f>
         <v>0.1427507995452611</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="8">
         <f t="shared" si="4"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="8">
         <f t="shared" si="4"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="8">
         <f t="shared" si="4"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="M14" t="s">
-        <v>73</v>
-      </c>
-      <c r="N14" t="s">
-        <v>72</v>
-      </c>
-      <c r="O14">
+      <c r="L14" s="5"/>
+      <c r="M14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O14" s="5">
         <f t="shared" si="2"/>
         <v>2.8550159909052221E-2</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="5">
         <f t="shared" si="3"/>
         <v>0.71375399772630543</v>
       </c>
-      <c r="Q14" t="s">
-        <v>73</v>
-      </c>
-      <c r="R14">
+      <c r="Q14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R14" s="5">
         <v>1.427507995452611E-2</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="10">
         <v>1.4275079954526109</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="8">
         <v>0.1427507995452611</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="M15" t="s">
-        <v>73</v>
-      </c>
-      <c r="N15" t="s">
-        <v>72</v>
-      </c>
-      <c r="O15">
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O15" s="5">
         <f t="shared" si="2"/>
         <v>2.8550159909052221E-2</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="5">
         <f t="shared" si="3"/>
         <v>0.71375399772630543</v>
       </c>
-      <c r="Q15" t="s">
-        <v>73</v>
-      </c>
-      <c r="R15">
+      <c r="Q15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R15" s="5">
         <v>1.427507995452611E-2</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="10">
         <v>1.4275079954526109</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="8">
         <v>0.2502723352076287</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="M16" t="s">
-        <v>72</v>
-      </c>
-      <c r="N16" t="s">
-        <v>73</v>
-      </c>
-      <c r="O16" s="5">
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O16" s="4">
         <f t="shared" ref="O16:O18" si="5">E16/10</f>
         <v>2.502723352076287E-2</v>
       </c>
-      <c r="P16" s="5">
+      <c r="P16" s="4">
         <f>E16*5</f>
         <v>1.2513616760381434</v>
       </c>
-      <c r="Q16" t="s">
-        <v>72</v>
-      </c>
-      <c r="R16">
+      <c r="Q16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R16" s="5">
         <v>2.502723352076287E-2</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="10">
         <v>2.5027233520762868</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="8">
         <v>0.2502723352076287</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="M17" t="s">
-        <v>72</v>
-      </c>
-      <c r="N17" t="s">
-        <v>73</v>
-      </c>
-      <c r="O17" s="5">
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O17" s="4">
         <f t="shared" si="5"/>
         <v>2.502723352076287E-2</v>
       </c>
-      <c r="P17" s="5">
+      <c r="P17" s="4">
         <f t="shared" ref="P17:P18" si="6">E17*5</f>
         <v>1.2513616760381434</v>
       </c>
-      <c r="Q17" t="s">
-        <v>72</v>
-      </c>
-      <c r="R17">
+      <c r="Q17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R17" s="5">
         <v>2.502723352076287E-2</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="10">
         <v>2.5027233520762868</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="8">
         <v>0.2502723352076287</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="M18" t="s">
-        <v>72</v>
-      </c>
-      <c r="N18" t="s">
-        <v>73</v>
-      </c>
-      <c r="O18" s="5">
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O18" s="4">
         <f t="shared" si="5"/>
         <v>2.502723352076287E-2</v>
       </c>
-      <c r="P18" s="5">
+      <c r="P18" s="4">
         <f t="shared" si="6"/>
         <v>1.2513616760381434</v>
       </c>
-      <c r="Q18" t="s">
-        <v>72</v>
-      </c>
-      <c r="R18">
+      <c r="Q18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="R18" s="5">
         <v>2.502723352076287E-2</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="10">
         <v>2.5027233520762868</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="8">
         <v>0.2502723352076287</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" t="s">
-        <v>72</v>
-      </c>
-      <c r="N19" t="s">
-        <v>72</v>
-      </c>
-      <c r="O19">
+      <c r="F19" s="5"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O19" s="5">
         <f t="shared" si="2"/>
         <v>5.005446704152574E-2</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="5">
         <f t="shared" si="3"/>
         <v>1.2513616760381434</v>
       </c>
-      <c r="Q19" t="s">
-        <v>73</v>
-      </c>
-      <c r="R19">
+      <c r="Q19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R19" s="5">
         <v>2.502723352076287E-2</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="10">
         <v>2.5027233520762868</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="4">
         <f>E21/5</f>
         <v>1.6399999999999999E-5</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="5">
         <f t="shared" si="0"/>
         <v>1.41696</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="M20" t="s">
-        <v>73</v>
-      </c>
-      <c r="N20" t="s">
-        <v>72</v>
-      </c>
-      <c r="O20">
+      <c r="G20" s="5">
+        <v>0</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5">
+        <v>0</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O20" s="5">
         <f t="shared" si="2"/>
         <v>3.2799999999999999E-6</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="5">
         <f t="shared" si="3"/>
         <v>8.1999999999999987E-5</v>
       </c>
-      <c r="Q20" t="s">
-        <v>73</v>
-      </c>
-      <c r="R20">
+      <c r="Q20" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R20" s="5">
         <v>1.64E-6</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="10">
         <v>1.6399999999999997E-4</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="4">
         <v>8.2000000000000001E-5</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="5">
         <f t="shared" si="0"/>
         <v>7.0848000000000004</v>
       </c>
-      <c r="M21" t="s">
-        <v>73</v>
-      </c>
-      <c r="N21" t="s">
-        <v>72</v>
-      </c>
-      <c r="O21">
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O21" s="5">
         <f t="shared" si="2"/>
         <v>1.6399999999999999E-5</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="5">
         <f t="shared" si="3"/>
         <v>4.0999999999999999E-4</v>
       </c>
-      <c r="Q21" t="s">
-        <v>73</v>
-      </c>
-      <c r="R21">
+      <c r="Q21" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R21" s="5">
         <v>8.1999999999999994E-6</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="10">
         <v>8.1999999999999998E-4</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="4">
         <f>E23/5</f>
         <v>1.2799999999999999E-5</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="5">
         <f t="shared" si="0"/>
         <v>1.1059199999999998</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="M22" t="s">
-        <v>73</v>
-      </c>
-      <c r="N22" t="s">
-        <v>72</v>
-      </c>
-      <c r="O22">
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0</v>
+      </c>
+      <c r="K22" s="5">
+        <v>0</v>
+      </c>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O22" s="5">
         <f t="shared" si="2"/>
         <v>2.5600000000000001E-6</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="5">
         <f t="shared" si="3"/>
         <v>6.3999999999999997E-5</v>
       </c>
-      <c r="Q22" t="s">
-        <v>73</v>
-      </c>
-      <c r="R22">
+      <c r="Q22" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R22" s="5">
         <v>1.28E-6</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="10">
         <v>1.2799999999999999E-4</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="4">
         <v>6.3999999999999997E-5</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="5">
         <f t="shared" si="0"/>
         <v>5.5296000000000003</v>
       </c>
-      <c r="M23" t="s">
-        <v>73</v>
-      </c>
-      <c r="N23" t="s">
-        <v>72</v>
-      </c>
-      <c r="O23">
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O23" s="5">
         <f t="shared" si="2"/>
         <v>1.2799999999999999E-5</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="5">
         <f t="shared" si="3"/>
         <v>3.1999999999999997E-4</v>
       </c>
-      <c r="Q23" t="s">
-        <v>73</v>
-      </c>
-      <c r="R23">
+      <c r="Q23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R23" s="5">
         <v>6.3999999999999997E-6</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="10">
         <v>6.3999999999999994E-4</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="4">
         <v>1.50462962962963E-5</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="5">
         <f t="shared" si="0"/>
         <v>1.3000000000000003</v>
       </c>
-      <c r="M24" t="s">
-        <v>72</v>
-      </c>
-      <c r="N24" t="s">
-        <v>73</v>
-      </c>
-      <c r="O24" s="5">
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O24" s="4">
         <f t="shared" ref="O24:O26" si="7">E24/10</f>
         <v>1.5046296296296301E-6</v>
       </c>
-      <c r="P24" s="5">
+      <c r="P24" s="4">
         <f t="shared" ref="P24:P26" si="8">E24*10</f>
         <v>1.50462962962963E-4</v>
       </c>
-      <c r="Q24" t="s">
-        <v>73</v>
-      </c>
-      <c r="R24">
+      <c r="Q24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R24" s="5">
         <v>1.5046296296296301E-6</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="10">
         <v>1.50462962962963E-4</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="4">
         <v>1.50462962962963E-5</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="5">
         <f t="shared" si="0"/>
         <v>1.3000000000000003</v>
       </c>
-      <c r="M25" t="s">
-        <v>72</v>
-      </c>
-      <c r="N25" t="s">
-        <v>73</v>
-      </c>
-      <c r="O25" s="5">
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O25" s="4">
         <f t="shared" si="7"/>
         <v>1.5046296296296301E-6</v>
       </c>
-      <c r="P25" s="5">
+      <c r="P25" s="4">
         <f t="shared" si="8"/>
         <v>1.50462962962963E-4</v>
       </c>
-      <c r="Q25" t="s">
-        <v>73</v>
-      </c>
-      <c r="R25">
+      <c r="Q25" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R25" s="5">
         <v>1.5046296296296301E-6</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="10">
         <v>1.50462962962963E-4</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="4">
         <v>6.7708333333333344E-5</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="5">
         <f t="shared" si="0"/>
         <v>5.8500000000000014</v>
       </c>
-      <c r="M26" t="s">
-        <v>72</v>
-      </c>
-      <c r="N26" t="s">
-        <v>73</v>
-      </c>
-      <c r="O26" s="5">
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O26" s="4">
         <f t="shared" si="7"/>
         <v>6.7708333333333347E-6</v>
       </c>
-      <c r="P26" s="5">
+      <c r="P26" s="4">
         <f t="shared" si="8"/>
         <v>6.7708333333333346E-4</v>
       </c>
-      <c r="Q26" t="s">
-        <v>73</v>
-      </c>
-      <c r="R26">
+      <c r="Q26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R26" s="5">
         <v>6.7708333333333347E-6</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="10">
         <v>6.7708333333333346E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E27" s="20">
-        <v>0</v>
-      </c>
-      <c r="F27" s="21">
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M27" t="s">
-        <v>72</v>
-      </c>
-      <c r="N27" t="s">
-        <v>72</v>
-      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N27" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="10"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="5">
         <v>1</v>
       </c>
-      <c r="F28" s="15"/>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
+      <c r="F28" s="5"/>
+      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+      <c r="H28" s="5">
         <v>1</v>
       </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0</v>
+      </c>
+      <c r="K28" s="5">
         <v>1</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-      <c r="M28" t="s">
-        <v>72</v>
-      </c>
-      <c r="N28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+      <c r="L28" s="5">
+        <v>0</v>
+      </c>
+      <c r="M28" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="10"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D29" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="5">
         <v>1</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
+      <c r="F29" s="5"/>
+      <c r="G29" s="5">
+        <v>0</v>
+      </c>
+      <c r="H29" s="5">
         <v>1</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
+      <c r="I29" s="5">
+        <v>0</v>
+      </c>
+      <c r="J29" s="5">
+        <v>0</v>
+      </c>
+      <c r="K29" s="5">
         <v>1</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29" t="s">
-        <v>72</v>
-      </c>
-      <c r="N29" t="s">
-        <v>72</v>
-      </c>
+      <c r="L29" s="5">
+        <v>0</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="10"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="4">
         <v>6.4814814814814812E-7</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="5">
         <f t="shared" si="0"/>
         <v>5.5999999999999994E-2</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30" t="s">
-        <v>73</v>
-      </c>
-      <c r="N30" t="s">
-        <v>72</v>
-      </c>
-      <c r="O30" s="5">
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="5">
+        <v>0</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5">
+        <v>0</v>
+      </c>
+      <c r="L30" s="5">
+        <v>0</v>
+      </c>
+      <c r="M30" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N30" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O30" s="4">
         <f t="shared" ref="O30:O33" si="9">E30/10</f>
         <v>6.4814814814814807E-8</v>
       </c>
-      <c r="P30" s="5">
+      <c r="P30" s="4">
         <f t="shared" ref="P30:P32" si="10">E30*10</f>
         <v>6.4814814814814812E-6</v>
       </c>
-      <c r="Q30" t="s">
-        <v>73</v>
-      </c>
-      <c r="R30">
+      <c r="Q30" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R30" s="5">
         <v>6.4814814814814807E-8</v>
       </c>
-      <c r="S30">
+      <c r="S30" s="10">
         <v>6.4814814814814812E-6</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -2361,57 +2476,58 @@
       <c r="D31" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="4">
         <v>4.0509259259259258E-7</v>
       </c>
-      <c r="F31" s="17">
+      <c r="F31" s="5">
         <f t="shared" si="0"/>
         <v>3.4999999999999996E-2</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31" t="s">
-        <v>72</v>
-      </c>
-      <c r="N31" t="s">
-        <v>73</v>
-      </c>
-      <c r="O31" s="5">
+      <c r="G31" s="5">
+        <v>0</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0</v>
+      </c>
+      <c r="I31" s="5">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5">
+        <v>0</v>
+      </c>
+      <c r="L31" s="5">
+        <v>0</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O31" s="4">
         <f t="shared" si="9"/>
         <v>4.0509259259259258E-8</v>
       </c>
-      <c r="P31" s="5">
+      <c r="P31" s="4">
         <f t="shared" si="10"/>
         <v>4.050925925925926E-6</v>
       </c>
-      <c r="Q31" t="s">
-        <v>73</v>
-      </c>
-      <c r="R31">
+      <c r="Q31" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R31" s="5">
         <v>4.0509259259259258E-8</v>
       </c>
-      <c r="S31">
+      <c r="S31" s="10">
         <v>4.050925925925926E-6</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -2420,184 +2536,185 @@
       <c r="D32" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="4">
         <v>7.6967592592592601E-6</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F32" s="5">
         <f t="shared" si="0"/>
         <v>0.66500000000000004</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32" t="s">
-        <v>72</v>
-      </c>
-      <c r="N32" t="s">
-        <v>73</v>
-      </c>
-      <c r="O32" s="5">
+      <c r="G32" s="5">
+        <v>0</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0</v>
+      </c>
+      <c r="I32" s="5">
+        <v>0</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5">
+        <v>0</v>
+      </c>
+      <c r="L32" s="5">
+        <v>0</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O32" s="4">
         <f t="shared" si="9"/>
         <v>7.6967592592592605E-7</v>
       </c>
-      <c r="P32" s="5">
+      <c r="P32" s="4">
         <f t="shared" si="10"/>
         <v>7.6967592592592601E-5</v>
       </c>
-      <c r="Q32" t="s">
-        <v>73</v>
-      </c>
-      <c r="R32">
+      <c r="Q32" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R32" s="5">
         <v>7.6967592592592605E-7</v>
       </c>
-      <c r="S32">
+      <c r="S32" s="10">
         <v>7.6967592592592601E-5</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="8">
         <v>0.2502723352076287</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="4">
+      <c r="F33" s="5"/>
+      <c r="G33" s="8">
         <f>$E33</f>
         <v>0.2502723352076287</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="8">
         <f t="shared" ref="H33:L33" si="11">$E33</f>
         <v>0.2502723352076287</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="8">
         <f t="shared" si="11"/>
         <v>0.2502723352076287</v>
       </c>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4">
+      <c r="J33" s="8"/>
+      <c r="K33" s="8">
         <f t="shared" si="11"/>
         <v>0.2502723352076287</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33" s="8">
         <f t="shared" si="11"/>
         <v>0.2502723352076287</v>
       </c>
-      <c r="M33" t="s">
-        <v>72</v>
-      </c>
-      <c r="N33" t="s">
-        <v>73</v>
-      </c>
-      <c r="O33" s="5">
+      <c r="M33" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O33" s="4">
         <f t="shared" si="9"/>
         <v>2.502723352076287E-2</v>
       </c>
-      <c r="P33" s="5">
+      <c r="P33" s="4">
         <f>E33*5</f>
         <v>1.2513616760381434</v>
       </c>
-      <c r="Q33" t="s">
-        <v>73</v>
-      </c>
-      <c r="R33">
+      <c r="Q33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R33" s="5">
         <v>2.502723352076287E-2</v>
       </c>
-      <c r="S33">
+      <c r="S33" s="10">
         <v>2.5027233520762868</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E34" s="20">
+      <c r="E34" s="5">
         <f>0.01/3600/24</f>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="F34" s="21">
+      <c r="F34" s="5">
         <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="5">
         <f>$E34</f>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="5">
         <f t="shared" ref="H34:L34" si="12">$E34</f>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="5">
         <f t="shared" si="12"/>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="5">
         <f t="shared" si="12"/>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="5">
         <f t="shared" si="12"/>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="5">
         <f t="shared" si="12"/>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="M34" t="s">
-        <v>73</v>
-      </c>
-      <c r="N34" t="s">
-        <v>72</v>
-      </c>
-      <c r="O34" s="5">
-        <v>0</v>
-      </c>
-      <c r="P34" s="5">
+      <c r="M34" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O34" s="4">
+        <v>0</v>
+      </c>
+      <c r="P34" s="4">
         <f t="shared" ref="P34:P45" si="13">E34*10</f>
         <v>1.1574074074074074E-6</v>
       </c>
-      <c r="Q34" t="s">
-        <v>73</v>
-      </c>
-      <c r="R34">
-        <v>0</v>
-      </c>
-      <c r="S34">
+      <c r="Q34" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R34" s="5">
+        <v>0</v>
+      </c>
+      <c r="S34" s="10">
         <v>1.1574074074074074E-6</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="26" t="s">
         <v>111</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2609,276 +2726,306 @@
       <c r="D35" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="4">
         <v>1.1574074074074101E-7</v>
       </c>
-      <c r="F35" s="17">
+      <c r="F35" s="5">
         <f>E35*3600*24</f>
         <v>1.0000000000000023E-2</v>
       </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35" t="s">
-        <v>73</v>
-      </c>
-      <c r="N35" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="G35" s="5">
+        <v>0</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0</v>
+      </c>
+      <c r="I35" s="5">
+        <v>0</v>
+      </c>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5">
+        <v>0</v>
+      </c>
+      <c r="L35" s="5">
+        <v>0</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="10"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E36" s="26">
+      <c r="E36" s="4">
         <v>1.1574074074074101E-7</v>
       </c>
-      <c r="F36" s="21">
+      <c r="F36" s="5">
         <f>E36*3600*24</f>
         <v>1.0000000000000023E-2</v>
       </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
-      <c r="M36" t="s">
-        <v>72</v>
-      </c>
-      <c r="N36" t="s">
-        <v>73</v>
-      </c>
+      <c r="G36" s="5">
+        <v>0</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+      <c r="I36" s="5">
+        <v>0</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5">
+        <v>0</v>
+      </c>
+      <c r="L36" s="5">
+        <v>0</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="10"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="8">
         <v>0.1427507995452611</v>
       </c>
-      <c r="M37" t="s">
-        <v>73</v>
-      </c>
-      <c r="N37" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="10"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="8">
         <v>0.1427507995452611</v>
       </c>
-      <c r="G38" s="4">
+      <c r="F38" s="5"/>
+      <c r="G38" s="8">
         <f>$E38</f>
         <v>0.1427507995452611</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="8">
         <f t="shared" ref="H38:L38" si="14">$E38</f>
         <v>0.1427507995452611</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="8">
         <f t="shared" si="14"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4">
+      <c r="J38" s="8"/>
+      <c r="K38" s="8">
         <f t="shared" si="14"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38" s="8">
         <f t="shared" si="14"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="M38" t="s">
-        <v>72</v>
-      </c>
-      <c r="N38" t="s">
-        <v>73</v>
-      </c>
+      <c r="M38" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N38" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="10"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="8">
         <v>0.1427507995452611</v>
       </c>
-      <c r="F39" s="15"/>
-      <c r="G39">
+      <c r="F39" s="5"/>
+      <c r="G39" s="5">
         <f t="shared" ref="G39:L40" si="15">$E39</f>
         <v>0.1427507995452611</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="5">
         <f t="shared" si="15"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="5">
         <f t="shared" si="15"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="5">
         <f t="shared" si="15"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="5">
         <f t="shared" si="15"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="5">
         <f t="shared" si="15"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="M39" t="s">
-        <v>73</v>
-      </c>
-      <c r="N39" t="s">
-        <v>72</v>
-      </c>
-      <c r="O39" s="5">
+      <c r="M39" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O39" s="4">
         <f t="shared" ref="O39:O45" si="16">E39/10</f>
         <v>1.427507995452611E-2</v>
       </c>
-      <c r="P39" s="5">
+      <c r="P39" s="4">
         <f t="shared" si="13"/>
         <v>1.4275079954526109</v>
       </c>
-      <c r="Q39" t="s">
-        <v>73</v>
-      </c>
-      <c r="R39">
+      <c r="Q39" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R39" s="5">
         <v>1.427507995452611E-2</v>
       </c>
-      <c r="S39">
+      <c r="S39" s="10">
         <v>1.4275079954526109</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="8">
         <v>0.1427507995452611</v>
       </c>
-      <c r="F40" s="17"/>
-      <c r="G40">
+      <c r="F40" s="5"/>
+      <c r="G40" s="5">
         <f t="shared" si="15"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="5">
         <f t="shared" si="15"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="5">
         <f t="shared" si="15"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="5">
         <f t="shared" si="15"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="5">
         <f t="shared" si="15"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="5">
         <f t="shared" si="15"/>
         <v>0.1427507995452611</v>
       </c>
-      <c r="M40" t="s">
-        <v>72</v>
-      </c>
-      <c r="N40" t="s">
-        <v>72</v>
-      </c>
-      <c r="O40" s="5">
+      <c r="M40" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O40" s="4">
         <f>E40/10</f>
         <v>1.427507995452611E-2</v>
       </c>
-      <c r="P40" s="5">
+      <c r="P40" s="4">
         <f>E40*10</f>
         <v>1.4275079954526109</v>
       </c>
-      <c r="Q40" t="s">
-        <v>73</v>
-      </c>
-      <c r="R40">
+      <c r="Q40" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R40" s="5">
         <v>1.427507995452611E-2</v>
       </c>
-      <c r="S40">
+      <c r="S40" s="10">
         <v>1.4275079954526109</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2890,57 +3037,57 @@
       <c r="D41" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="4">
         <v>6.4814814814814799E-17</v>
       </c>
-      <c r="F41" s="17">
+      <c r="F41" s="5">
         <f t="shared" si="0"/>
         <v>5.5999999999999988E-12</v>
       </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>0</v>
-      </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-      <c r="M41" t="s">
-        <v>73</v>
-      </c>
-      <c r="N41" t="s">
-        <v>72</v>
-      </c>
-      <c r="O41" s="5">
+      <c r="G41" s="5">
+        <v>0</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0</v>
+      </c>
+      <c r="I41" s="5">
+        <v>0</v>
+      </c>
+      <c r="J41" s="5">
+        <v>0</v>
+      </c>
+      <c r="K41" s="5">
+        <v>0</v>
+      </c>
+      <c r="L41" s="5">
+        <v>0</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N41" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O41" s="4">
         <f t="shared" si="16"/>
         <v>6.4814814814814798E-18</v>
       </c>
-      <c r="P41" s="5">
+      <c r="P41" s="4">
         <f t="shared" si="13"/>
         <v>6.4814814814814797E-16</v>
       </c>
-      <c r="Q41" t="s">
-        <v>73</v>
-      </c>
-      <c r="R41">
+      <c r="Q41" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R41" s="5">
         <v>6.4814814814814798E-18</v>
       </c>
-      <c r="S41">
+      <c r="S41" s="10">
         <v>6.4814814814814797E-16</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -2952,57 +3099,57 @@
       <c r="D42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="4">
         <v>4.0509259259259248E-17</v>
       </c>
-      <c r="F42" s="17">
+      <c r="F42" s="5">
         <f t="shared" si="0"/>
         <v>3.4999999999999988E-12</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-      <c r="M42" t="s">
-        <v>72</v>
-      </c>
-      <c r="N42" t="s">
-        <v>72</v>
-      </c>
-      <c r="O42" s="5">
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0</v>
+      </c>
+      <c r="I42" s="5">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5">
+        <v>0</v>
+      </c>
+      <c r="K42" s="5">
+        <v>0</v>
+      </c>
+      <c r="L42" s="5">
+        <v>0</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N42" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O42" s="4">
         <f t="shared" si="16"/>
         <v>4.050925925925925E-18</v>
       </c>
-      <c r="P42" s="5">
+      <c r="P42" s="4">
         <f t="shared" si="13"/>
         <v>4.0509259259259247E-16</v>
       </c>
-      <c r="Q42" t="s">
-        <v>73</v>
-      </c>
-      <c r="R42">
+      <c r="Q42" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R42" s="5">
         <v>4.050925925925925E-18</v>
       </c>
-      <c r="S42">
+      <c r="S42" s="10">
         <v>4.0509259259259247E-16</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="16" t="s">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -3011,63 +3158,63 @@
       <c r="C43" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D43" s="32" t="s">
+      <c r="D43" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E43" s="20">
+      <c r="E43" s="5">
         <f>0.01/3600/24</f>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="F43" s="17">
+      <c r="F43" s="5">
         <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43" s="4">
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0</v>
+      </c>
+      <c r="I43" s="5">
+        <v>0</v>
+      </c>
+      <c r="J43" s="5">
+        <v>0</v>
+      </c>
+      <c r="K43" s="8">
         <f>E43</f>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L43" s="8">
         <f>E43</f>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="M43" t="s">
-        <v>72</v>
-      </c>
-      <c r="N43" t="s">
-        <v>72</v>
-      </c>
-      <c r="O43" s="5">
+      <c r="M43" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N43" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O43" s="4">
         <f t="shared" si="16"/>
         <v>1.1574074074074074E-8</v>
       </c>
-      <c r="P43" s="5">
+      <c r="P43" s="4">
         <f t="shared" si="13"/>
         <v>1.1574074074074074E-6</v>
       </c>
-      <c r="Q43" t="s">
-        <v>73</v>
-      </c>
-      <c r="R43">
+      <c r="Q43" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R43" s="5">
         <v>1.1574074074074074E-8</v>
       </c>
-      <c r="S43">
+      <c r="S43" s="10">
         <v>1.1574074074074074E-6</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="16" t="s">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -3076,63 +3223,63 @@
       <c r="C44" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D44" s="32" t="s">
+      <c r="D44" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E44" s="20">
+      <c r="E44" s="5">
         <f>0.01/3600/24</f>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="F44" s="17">
+      <c r="F44" s="5">
         <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44" s="4">
+      <c r="G44" s="5">
+        <v>0</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0</v>
+      </c>
+      <c r="I44" s="5">
+        <v>0</v>
+      </c>
+      <c r="J44" s="5">
+        <v>0</v>
+      </c>
+      <c r="K44" s="8">
         <f>E44</f>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="L44" s="4">
+      <c r="L44" s="8">
         <f>E44</f>
         <v>1.1574074074074074E-7</v>
       </c>
-      <c r="M44" t="s">
-        <v>72</v>
-      </c>
-      <c r="N44" t="s">
-        <v>72</v>
-      </c>
-      <c r="O44" s="5">
+      <c r="M44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O44" s="4">
         <f t="shared" si="16"/>
         <v>1.1574074074074074E-8</v>
       </c>
-      <c r="P44" s="5">
+      <c r="P44" s="4">
         <f t="shared" si="13"/>
         <v>1.1574074074074074E-6</v>
       </c>
-      <c r="Q44" t="s">
-        <v>73</v>
-      </c>
-      <c r="R44">
+      <c r="Q44" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R44" s="5">
         <v>1.1574074074074074E-8</v>
       </c>
-      <c r="S44">
+      <c r="S44" s="10">
         <v>1.1574074074074074E-6</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="9" t="s">
         <v>38</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -3144,119 +3291,119 @@
       <c r="D45" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="4">
         <v>1.1574074074074101E-7</v>
       </c>
-      <c r="F45" s="17">
+      <c r="F45" s="5">
         <f t="shared" si="0"/>
         <v>1.0000000000000023E-2</v>
       </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-      <c r="M45" t="s">
-        <v>72</v>
-      </c>
-      <c r="N45" t="s">
-        <v>72</v>
-      </c>
-      <c r="O45" s="5">
+      <c r="G45" s="5">
+        <v>0</v>
+      </c>
+      <c r="H45" s="5">
+        <v>0</v>
+      </c>
+      <c r="I45" s="5">
+        <v>0</v>
+      </c>
+      <c r="J45" s="5">
+        <v>0</v>
+      </c>
+      <c r="K45" s="5">
+        <v>0</v>
+      </c>
+      <c r="L45" s="5">
+        <v>0</v>
+      </c>
+      <c r="M45" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N45" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O45" s="4">
         <f t="shared" si="16"/>
         <v>1.15740740740741E-8</v>
       </c>
-      <c r="P45" s="5">
+      <c r="P45" s="4">
         <f t="shared" si="13"/>
         <v>1.1574074074074101E-6</v>
       </c>
-      <c r="Q45" t="s">
-        <v>73</v>
-      </c>
-      <c r="R45">
+      <c r="Q45" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R45" s="5">
         <v>1.15740740740741E-8</v>
       </c>
-      <c r="S45">
+      <c r="S45" s="10">
         <v>1.1574074074074101E-6</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="18" t="s">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D46" s="19" t="s">
+      <c r="D46" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E46" s="26">
+      <c r="E46" s="4">
         <v>1.1574074074074101E-7</v>
       </c>
-      <c r="F46" s="21">
+      <c r="F46" s="5">
         <f t="shared" si="0"/>
         <v>1.0000000000000023E-2</v>
       </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <v>0</v>
-      </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
-      <c r="K46">
-        <v>0</v>
-      </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
-      <c r="M46" t="s">
-        <v>72</v>
-      </c>
-      <c r="N46" t="s">
-        <v>72</v>
-      </c>
-      <c r="O46" s="5">
+      <c r="G46" s="5">
+        <v>0</v>
+      </c>
+      <c r="H46" s="5">
+        <v>0</v>
+      </c>
+      <c r="I46" s="5">
+        <v>0</v>
+      </c>
+      <c r="J46" s="5">
+        <v>0</v>
+      </c>
+      <c r="K46" s="5">
+        <v>0</v>
+      </c>
+      <c r="L46" s="5">
+        <v>0</v>
+      </c>
+      <c r="M46" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N46" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O46" s="4">
         <f>E46/10</f>
         <v>1.15740740740741E-8</v>
       </c>
-      <c r="P46" s="5">
+      <c r="P46" s="4">
         <f>E46*10</f>
         <v>1.1574074074074101E-6</v>
       </c>
-      <c r="Q46" t="s">
-        <v>73</v>
-      </c>
-      <c r="R46">
+      <c r="Q46" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="R46" s="5">
         <v>1.15740740740741E-8</v>
       </c>
-      <c r="S46">
+      <c r="S46" s="10">
         <v>1.1574074074074101E-6</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="9" t="s">
         <v>40</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -3268,22 +3415,33 @@
       <c r="D47" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="4">
         <v>2.083333333333333E-6</v>
       </c>
-      <c r="F47" s="17">
+      <c r="F47" s="5">
         <f t="shared" si="0"/>
         <v>0.17999999999999997</v>
       </c>
-      <c r="M47" t="s">
-        <v>72</v>
-      </c>
-      <c r="N47" t="s">
-        <v>72</v>
-      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N47" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="10"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -3295,22 +3453,33 @@
       <c r="D48" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="4">
         <v>2.083333333333333E-6</v>
       </c>
-      <c r="F48" s="17">
+      <c r="F48" s="5">
         <f t="shared" si="0"/>
         <v>0.17999999999999997</v>
       </c>
-      <c r="M48" t="s">
-        <v>72</v>
-      </c>
-      <c r="N48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="s">
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N48" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="10"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -3322,270 +3491,374 @@
       <c r="D49" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E49" s="5">
         <v>0.01</v>
       </c>
-      <c r="F49" s="17"/>
-      <c r="M49" t="s">
-        <v>72</v>
-      </c>
-      <c r="N49" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="18" t="s">
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N49" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="5"/>
+      <c r="S49" s="10"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="19" t="s">
+      <c r="D50" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="20">
+      <c r="E50" s="5">
         <v>0.01</v>
       </c>
-      <c r="F50" s="21"/>
-      <c r="M50" t="s">
-        <v>72</v>
-      </c>
-      <c r="N50" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N50" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="10"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="5">
         <v>0.25</v>
       </c>
-      <c r="M51" t="s">
-        <v>72</v>
-      </c>
-      <c r="N51" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="5"/>
+      <c r="S51" s="10"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="5">
         <v>0.1</v>
       </c>
-      <c r="M52" t="s">
-        <v>72</v>
-      </c>
-      <c r="N52" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="10"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="5">
         <v>0.25</v>
       </c>
-      <c r="M53" t="s">
-        <v>72</v>
-      </c>
-      <c r="N53" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N53" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="10"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="5">
         <v>0.1</v>
       </c>
-      <c r="M54" t="s">
-        <v>72</v>
-      </c>
-      <c r="N54" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="5"/>
+      <c r="S54" s="10"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55" s="4">
         <v>3.4999999999999997E-5</v>
       </c>
-      <c r="F55" s="17">
+      <c r="F55" s="5">
         <f t="shared" ref="F55:F56" si="17">E55*3600*24</f>
         <v>3.024</v>
       </c>
-      <c r="M55" t="s">
-        <v>72</v>
-      </c>
-      <c r="N55" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N55" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="5"/>
+      <c r="S55" s="10"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E56" s="5">
+      <c r="E56" s="4">
         <v>3.4999999999999997E-5</v>
       </c>
-      <c r="F56" s="17">
+      <c r="F56" s="5">
         <f t="shared" si="17"/>
         <v>3.024</v>
       </c>
-      <c r="M56" t="s">
-        <v>72</v>
-      </c>
-      <c r="N56" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N56" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="5"/>
+      <c r="S56" s="10"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A57" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="7" t="s">
         <v>120</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57" s="4">
         <v>1.1574074074074101E-7</v>
       </c>
-      <c r="F57" s="17">
+      <c r="F57" s="5">
         <f t="shared" ref="F57:F58" si="18">E57*3600*24</f>
         <v>1.0000000000000023E-2</v>
       </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
-      <c r="K57">
-        <v>0</v>
-      </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-      <c r="M57" t="s">
-        <v>73</v>
-      </c>
-      <c r="N57" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
+      <c r="G57" s="5">
+        <v>0</v>
+      </c>
+      <c r="H57" s="5">
+        <v>0</v>
+      </c>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5">
+        <v>0</v>
+      </c>
+      <c r="K57" s="5">
+        <v>0</v>
+      </c>
+      <c r="L57" s="5">
+        <v>0</v>
+      </c>
+      <c r="M57" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="N57" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="5"/>
+      <c r="S57" s="10"/>
+    </row>
+    <row r="58" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="D58" s="19" t="s">
+      <c r="D58" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E58" s="26">
+      <c r="E58" s="14">
         <v>1.1574074074074101E-7</v>
       </c>
-      <c r="F58" s="21">
+      <c r="F58" s="12">
         <f t="shared" si="18"/>
         <v>1.0000000000000023E-2</v>
       </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
-      <c r="J58">
-        <v>0</v>
-      </c>
-      <c r="K58">
-        <v>0</v>
-      </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
-      <c r="M58" t="s">
-        <v>72</v>
-      </c>
-      <c r="N58" t="s">
-        <v>73</v>
-      </c>
+      <c r="G58" s="12">
+        <v>0</v>
+      </c>
+      <c r="H58" s="12">
+        <v>0</v>
+      </c>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12">
+        <v>0</v>
+      </c>
+      <c r="K58" s="12">
+        <v>0</v>
+      </c>
+      <c r="L58" s="12">
+        <v>0</v>
+      </c>
+      <c r="M58" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="N58" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="O58" s="12"/>
+      <c r="P58" s="12"/>
+      <c r="Q58" s="12"/>
+      <c r="R58" s="12"/>
+      <c r="S58" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:S58" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>